<commit_message>
INTERACTIVE MAP 0.3.0 change filter for date to range
</commit_message>
<xml_diff>
--- a/src/assets/resumen_variables.xlsx
+++ b/src/assets/resumen_variables.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>variable_name</t>
   </si>
@@ -81,13 +81,10 @@
     <t>Caudales observados en estaciones fluiométricas en la cuenca del río Maipo.</t>
   </si>
   <si>
-    <t>caudales_modelados_cord</t>
+    <t>caudales_modelados</t>
   </si>
   <si>
     <t>Caudal Modelado Cordillera</t>
-  </si>
-  <si>
-    <t>caudales_modelados</t>
   </si>
   <si>
     <r>
@@ -114,9 +111,6 @@
       </rPr>
       <t>/s]</t>
     </r>
-  </si>
-  <si>
-    <t>caudales_observados_cord</t>
   </si>
   <si>
     <t>Agua Potable Producida</t>
@@ -480,7 +474,7 @@
       <c r="E3" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -489,10 +483,10 @@
         <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>14</v>
@@ -500,22 +494,22 @@
       <c r="E4" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>19</v>
+      <c r="F4" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="E5" s="5" t="b">
         <v>1</v>

</xml_diff>